<commit_message>
Potion stuff very nearly done
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Artificing/ingredients.xlsx
+++ b/CoreRulebook/Data/Artificing/ingredients.xlsx
@@ -11,9 +11,9 @@
     <sheet name="ingredients" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ingredients!$A$1:$H$117</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ingredients!$A$1:$P$117</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">ingredients!$A$1:$P$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ingredients!$A$1:$P$119</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ingredients!$A$1:$H$119</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">ingredients!$A$1:$P$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="309">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -87,6 +87,9 @@
     <t xml:space="preserve">A powerfully acidic, foul smelling grey secretion.</t>
   </si>
   <si>
+    <t xml:space="preserve">Common</t>
+  </si>
+  <si>
     <t xml:space="preserve">Smelly</t>
   </si>
   <si>
@@ -240,9 +243,6 @@
     <t xml:space="preserve">The brilliant blue flower of a common, non-magical (but poisonous) plant.</t>
   </si>
   <si>
-    <t xml:space="preserve">Common</t>
-  </si>
-  <si>
     <t xml:space="preserve">Poisonous</t>
   </si>
   <si>
@@ -255,6 +255,9 @@
     <t xml:space="preserve">Consuming the speckled leaves of the `hyena tree\apos{} results in uncontrollable laughter</t>
   </si>
   <si>
+    <t xml:space="preserve">Unusual</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hallucinogenic</t>
   </si>
   <si>
@@ -264,16 +267,22 @@
     <t xml:space="preserve">The tail of a poisonois European snake, used in potion making for thousands of years.</t>
   </si>
   <si>
+    <t xml:space="preserve">Paralytic</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bezoar</t>
   </si>
   <si>
-    <t xml:space="preserve">A hard, brown lump formed in the stomach of a goat. </t>
+    <t xml:space="preserve">A hard, brown lump formed in the stomach of a goat. Horrifying to look at, but said to be a powerful antidote.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ugly</t>
   </si>
   <si>
     <t xml:space="preserve">Billywig Sting</t>
   </si>
   <si>
-    <t xml:space="preserve">The venom inside causes giddiness and levitation.</t>
+    <t xml:space="preserve">The venom inside this vicious barb causes giddiness and levitation.</t>
   </si>
   <si>
     <t xml:space="preserve">Boomberry</t>
@@ -291,9 +300,6 @@
     <t xml:space="preserve">White  sap from the magic tree causes boils on contact.</t>
   </si>
   <si>
-    <t xml:space="preserve">Paralytic</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bulbadox Powder</t>
   </si>
   <si>
@@ -345,6 +351,9 @@
     <t xml:space="preserve">Very dense wood-like material from the back of a dugbog.</t>
   </si>
   <si>
+    <t xml:space="preserve">Singular</t>
+  </si>
+  <si>
     <t xml:space="preserve">Resilient</t>
   </si>
   <si>
@@ -372,6 +381,27 @@
     <t xml:space="preserve">Flexible</t>
   </si>
   <si>
+    <t xml:space="preserve">Raiju Shaving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A clump of fur torn from the lightning-fast thunder dog, crackles with energy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accelerant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyclops Eye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The single eye torn from the thunder giant tribe, very rare and very dangerous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enraging</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hemlock Essence</t>
   </si>
   <si>
@@ -441,6 +471,9 @@
     <t xml:space="preserve">Glowing fluid that seems to calm you down just by looking at it.</t>
   </si>
   <si>
+    <t xml:space="preserve">Inspiring</t>
+  </si>
+  <si>
     <t xml:space="preserve">Murtlap Tentacles</t>
   </si>
   <si>
@@ -519,12 +552,6 @@
     <t xml:space="preserve">A brown, hairy leg from a magic abomination. Filled with hatred and power.</t>
   </si>
   <si>
-    <t xml:space="preserve">Enraging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ugly</t>
-  </si>
-  <si>
     <t xml:space="preserve">Acheron Water</t>
   </si>
   <si>
@@ -621,18 +648,12 @@
     <t xml:space="preserve">Radiant</t>
   </si>
   <si>
-    <t xml:space="preserve">Inspiring</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thunderbird Feather</t>
   </si>
   <si>
     <t xml:space="preserve">A pale, golden feather which seems to crackle with energy. Merely touching it causes your hair to stand on end. </t>
   </si>
   <si>
-    <t xml:space="preserve">Accelerant</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unicorn Blood</t>
   </si>
   <si>
@@ -651,9 +672,6 @@
     <t xml:space="preserve">A clutch of the eggs of a fire-snake. They are red-hot, and are renowned in love potions.</t>
   </si>
   <si>
-    <t xml:space="preserve">Rare</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bicorn Horn</t>
   </si>
   <si>
@@ -762,7 +780,7 @@
     <t xml:space="preserve">Sea-Serpent Spine</t>
   </si>
   <si>
-    <t xml:space="preserve">Shed from the fins of aquatic beasts, these spines are used by poisoners worldwide.</t>
+    <t xml:space="preserve">Shed from the fins of aquatic beasts, these spines are used by poisoners worldwide, and are renowned for their ability to pierce even the toughest materials. </t>
   </si>
   <si>
     <t xml:space="preserve">Abyssinian Shrivelfig</t>
@@ -771,9 +789,6 @@
     <t xml:space="preserve">A purple fruit found in the African desert. Dries up and shrinks when picked.</t>
   </si>
   <si>
-    <t xml:space="preserve">Singular</t>
-  </si>
-  <si>
     <t xml:space="preserve">Boomslang Skin</t>
   </si>
   <si>
@@ -901,9 +916,6 @@
   </si>
   <si>
     <t xml:space="preserve">The ice-cold blood of the frost salamander, a pleasant sky-blue colour.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unusual</t>
   </si>
   <si>
     <t xml:space="preserve">Hippocampus Hair</t>
@@ -1052,14 +1064,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ117"/>
+  <dimension ref="A1:AMJ119"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
-      <selection pane="bottomRight" activeCell="A63" activeCellId="0" sqref="A63"/>
+      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1156,129 +1168,129 @@
         <v>19</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>10</v>
@@ -1290,160 +1302,160 @@
         <v>17</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>72</v>
@@ -1460,52 +1472,58 @@
         <v>75</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>73</v>
@@ -1513,905 +1531,908 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>72</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>73</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>72</v>
+        <v>100</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>39</v>
+        <v>124</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>97</v>
+        <v>20</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>123</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>126</v>
+        <v>20</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>91</v>
+        <v>58</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>97</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>33</v>
+        <v>139</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F46" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="G46" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>73</v>
+        <v>17</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>91</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>106</v>
+        <v>21</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>103</v>
+        <v>61</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>156</v>
+        <v>20</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="F54" s="0" t="s">
-        <v>157</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>156</v>
+        <v>20</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>129</v>
+        <v>98</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>32</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>164</v>
+        <v>88</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="B58" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C58" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="C58" s="0" t="s">
-        <v>156</v>
-      </c>
       <c r="D58" s="0" t="s">
-        <v>168</v>
+        <v>26</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>88</v>
+        <v>27</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>171</v>
+        <v>139</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>172</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>176</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F60" s="0" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>178</v>
+        <v>77</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>85</v>
+        <v>180</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>106</v>
+        <v>184</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>181</v>
+        <v>43</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>22</v>
+        <v>187</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>88</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>189</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>32</v>
+        <v>190</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F65" s="0" t="s">
-        <v>88</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G67" s="0" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="D68" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="D70" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="E68" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F68" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="G68" s="0" t="s">
+      <c r="E70" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G70" s="0" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="F69" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="G69" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="H69" s="0" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="F70" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="G70" s="0" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>204</v>
+        <v>52</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>206</v>
+      </c>
+      <c r="H71" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>178</v>
+        <v>99</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2422,79 +2443,79 @@
         <v>210</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>29</v>
+        <v>211</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>171</v>
+        <v>33</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="F74" s="0" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>123</v>
+        <v>26</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>216</v>
+        <v>30</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G76" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="H76" s="0" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2505,412 +2526,421 @@
         <v>221</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>29</v>
+        <v>133</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F77" s="0" t="s">
-        <v>126</v>
+        <v>222</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>60</v>
+        <v>139</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="H78" s="0" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>98</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>26</v>
+        <v>187</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="F80" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G80" s="0" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
       <c r="E81" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F82" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F81" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="G81" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="H81" s="0" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E82" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="F82" s="0" t="s">
-        <v>97</v>
+      <c r="G82" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>211</v>
+        <v>12</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>68</v>
+        <v>187</v>
+      </c>
+      <c r="G83" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H83" s="0" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>181</v>
+        <v>225</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>205</v>
+        <v>30</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>129</v>
+        <v>217</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>129</v>
+        <v>212</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>211</v>
+        <v>139</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>208</v>
+        <v>76</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>181</v>
+        <v>217</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>248</v>
+        <v>123</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>248</v>
+        <v>123</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>91</v>
+        <v>190</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>248</v>
+        <v>76</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>178</v>
+        <v>69</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F94" s="0" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>181</v>
+        <v>72</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="F95" s="0" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="F96" s="0" t="s">
-        <v>126</v>
+        <v>52</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F97" s="0" t="s">
-        <v>126</v>
+        <v>44</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>32</v>
+        <v>180</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+      <c r="F98" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>266</v>
       </c>
@@ -2918,13 +2948,16 @@
         <v>267</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>106</v>
+        <v>80</v>
+      </c>
+      <c r="F99" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2935,212 +2968,215 @@
         <v>269</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>106</v>
+        <v>270</v>
       </c>
       <c r="F102" s="0" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>197</v>
+        <v>26</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>97</v>
+        <v>55</v>
+      </c>
+      <c r="F103" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>129</v>
+        <v>109</v>
+      </c>
+      <c r="F104" s="0" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="F105" s="0" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>103</v>
+        <v>187</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>139</v>
+      </c>
+      <c r="F107" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E109" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F109" s="0" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>248</v>
+        <v>20</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>211</v>
+        <v>23</v>
       </c>
       <c r="E110" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F110" s="0" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>292</v>
+        <v>108</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>172</v>
+        <v>114</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>42</v>
+        <v>17</v>
+      </c>
+      <c r="F111" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3151,16 +3187,16 @@
         <v>294</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>292</v>
+        <v>76</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>26</v>
+        <v>217</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F112" s="0" t="s">
-        <v>265</v>
+        <v>93</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3171,16 +3207,13 @@
         <v>296</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>292</v>
+        <v>76</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>76</v>
+        <v>181</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F113" s="0" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3191,13 +3224,16 @@
         <v>298</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>292</v>
+        <v>76</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>201</v>
+        <v>27</v>
       </c>
       <c r="E114" s="0" t="s">
-        <v>76</v>
+        <v>30</v>
+      </c>
+      <c r="F114" s="0" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3208,13 +3244,16 @@
         <v>300</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>292</v>
+        <v>76</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>171</v>
+        <v>30</v>
+      </c>
+      <c r="F115" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3225,13 +3264,13 @@
         <v>302</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>292</v>
+        <v>76</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3242,14 +3281,48 @@
         <v>304</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>292</v>
+        <v>76</v>
       </c>
       <c r="D117" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="E117" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D118" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E118" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D119" s="0" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H117"/>
+  <autoFilter ref="A1:P119"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>